<commit_message>
PID-Filter: add unit test for min/max limits
</commit_message>
<xml_diff>
--- a/io.openems.edge.common/doc/PID-Simulator.xlsx
+++ b/io.openems.edge.common/doc/PID-Simulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.feilmeier\fems\develop\io.openems.edge.common\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5029A7AE-F60B-46CB-8CEC-B54DFE60F30C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C59140D-9587-4D59-8070-DBE39633856C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulator" sheetId="1" r:id="rId1"/>
@@ -257,8 +257,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2257,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6254,7 +6254,7 @@
         <v>1</v>
       </c>
       <c r="N66" s="9">
-        <f t="shared" ref="N66:N97" ca="1" si="21">IF(M66,L66,IF(Min&gt;L66,Min,IF(Max&lt;L66,Max,L66)))</f>
+        <f t="shared" ref="N66:N72" ca="1" si="21">IF(M66,L66,IF(Min&gt;L66,Min,IF(Max&lt;L66,Max,L66)))</f>
         <v>20000.00166314518</v>
       </c>
     </row>
@@ -6615,7 +6615,7 @@
   <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>